<commit_message>
create timesheet management project and database
</commit_message>
<xml_diff>
--- a/Cham_cong.xlsx
+++ b/Cham_cong.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="42">
   <si>
     <t>BANG CHAM CONG</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Chuc vu</t>
   </si>
   <si>
-    <t>Ngay lam viec</t>
-  </si>
-  <si>
     <t>Nghi co phep</t>
   </si>
   <si>
@@ -132,9 +129,6 @@
     <t>NV</t>
   </si>
   <si>
-    <t>TP</t>
-  </si>
-  <si>
     <t>QL</t>
   </si>
   <si>
@@ -154,6 +148,9 @@
   </si>
   <si>
     <t>Tên nhân viên</t>
+  </si>
+  <si>
+    <t>Gio lam viec</t>
   </si>
 </sst>
 </file>
@@ -501,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM22"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -547,7 +544,7 @@
     <row r="1" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -745,16 +742,16 @@
       <c r="AH5" s="9"/>
       <c r="AI5" s="9"/>
       <c r="AJ5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AK5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="AK5" s="7" t="s">
+      <c r="AL5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="AL5" s="7" t="s">
+      <c r="AM5" s="8" t="s">
         <v>9</v>
-      </c>
-      <c r="AM5" s="8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:39" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -835,94 +832,94 @@
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="H7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="J7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K7" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="L7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="M7" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="N7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="O7" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="P7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="Q7" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="R7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="S7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S7" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="T7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="U7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="U7" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="V7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="W7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="W7" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="X7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="Y7" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="Z7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AA7" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="AB7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AC7" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="AD7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AE7" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="AF7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AG7" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="AH7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI7" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="AI7" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="AJ7" s="7"/>
       <c r="AK7" s="7"/>
@@ -935,13 +932,13 @@
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="2"/>
@@ -980,13 +977,13 @@
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="2"/>
@@ -1025,13 +1022,13 @@
         <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1070,13 +1067,13 @@
         <v>4</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
@@ -1115,13 +1112,13 @@
         <v>5</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1160,13 +1157,13 @@
         <v>6</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1205,13 +1202,13 @@
         <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1250,13 +1247,13 @@
         <v>8</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1295,13 +1292,13 @@
         <v>9</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -1340,13 +1337,13 @@
         <v>10</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1518,38 +1515,38 @@
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B1" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
         <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">

</xml_diff>